<commit_message>
fixed showing graphs for unavailable data
</commit_message>
<xml_diff>
--- a/data101_data/roof_and_wall_cleaned.xlsx
+++ b/data101_data/roof_and_wall_cleaned.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JUPYTER FILES\DATA101\Project\Final Project Dash App\D101_Interactive_Visualization_Project\data101_data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{165DF985-7AD3-4003-9538-98EA71D286B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="19140" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="115">
   <si>
     <t>Region</t>
   </si>
@@ -356,13 +362,16 @@
   </si>
   <si>
     <t>SURIGAO DEL SUR</t>
+  </si>
+  <si>
+    <t>NCR, CITY OF MANILA, FIRST DISTRICT (NOT A PROVINCE)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -425,13 +434,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -469,7 +486,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -503,6 +520,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -537,9 +555,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -712,14 +731,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K87"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -754,7 +775,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -789,7 +810,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -824,7 +845,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -859,7 +880,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -894,7 +915,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -929,7 +950,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -964,7 +985,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -999,7 +1020,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1034,7 +1055,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1069,7 +1090,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1104,7 +1125,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1139,7 +1160,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1174,7 +1195,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1209,7 +1230,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1244,7 +1265,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1279,7 +1300,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -1314,2453 +1335,2488 @@
         <v>131</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>114</v>
       </c>
       <c r="C18">
-        <v>760689</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>99717</v>
+        <v>0</v>
       </c>
       <c r="E18">
-        <v>659</v>
+        <v>0</v>
       </c>
       <c r="F18">
-        <v>477</v>
+        <v>0</v>
       </c>
       <c r="G18">
-        <v>3858</v>
+        <v>0</v>
       </c>
       <c r="H18">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="I18">
-        <v>168</v>
+        <v>0</v>
       </c>
       <c r="J18">
-        <v>795</v>
+        <v>0</v>
       </c>
       <c r="K18">
-        <v>1295</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C19">
-        <v>946598</v>
+        <v>760689</v>
       </c>
       <c r="D19">
-        <v>95004</v>
+        <v>99717</v>
       </c>
       <c r="E19">
-        <v>648</v>
+        <v>659</v>
       </c>
       <c r="F19">
-        <v>246</v>
+        <v>477</v>
       </c>
       <c r="G19">
-        <v>1620</v>
+        <v>3858</v>
       </c>
       <c r="H19">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="I19">
-        <v>447</v>
+        <v>168</v>
       </c>
       <c r="J19">
-        <v>778</v>
+        <v>795</v>
       </c>
       <c r="K19">
-        <v>1687</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
+        <v>1295</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>14</v>
       </c>
       <c r="B20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20">
+        <v>946598</v>
+      </c>
+      <c r="D20">
+        <v>95004</v>
+      </c>
+      <c r="E20">
+        <v>648</v>
+      </c>
+      <c r="F20">
+        <v>246</v>
+      </c>
+      <c r="G20">
+        <v>1620</v>
+      </c>
+      <c r="H20">
+        <v>115</v>
+      </c>
+      <c r="I20">
+        <v>447</v>
+      </c>
+      <c r="J20">
+        <v>778</v>
+      </c>
+      <c r="K20">
+        <v>1687</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" t="s">
         <v>46</v>
       </c>
-      <c r="C20">
+      <c r="C21">
         <v>569612</v>
       </c>
-      <c r="D20">
+      <c r="D21">
         <v>63469</v>
       </c>
-      <c r="E20">
+      <c r="E21">
         <v>509</v>
       </c>
-      <c r="F20">
+      <c r="F21">
         <v>211</v>
       </c>
-      <c r="G20">
+      <c r="G21">
         <v>1999</v>
       </c>
-      <c r="H20">
+      <c r="H21">
         <v>73</v>
       </c>
-      <c r="I20">
+      <c r="I21">
         <v>308</v>
       </c>
-      <c r="J20">
+      <c r="J21">
         <v>471</v>
       </c>
-      <c r="K20">
+      <c r="K21">
         <v>1099</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
-      <c r="A21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21">
-        <v>115041</v>
-      </c>
-      <c r="D21">
-        <v>10866</v>
-      </c>
-      <c r="E21">
-        <v>136</v>
-      </c>
-      <c r="F21">
-        <v>1070</v>
-      </c>
-      <c r="G21">
-        <v>3925</v>
-      </c>
-      <c r="H21">
-        <v>48</v>
-      </c>
-      <c r="I21">
-        <v>4</v>
-      </c>
-      <c r="J21">
-        <v>11</v>
-      </c>
-      <c r="K21">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>15</v>
       </c>
       <c r="B22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22">
+        <v>115041</v>
+      </c>
+      <c r="D22">
+        <v>10866</v>
+      </c>
+      <c r="E22">
+        <v>136</v>
+      </c>
+      <c r="F22">
+        <v>1070</v>
+      </c>
+      <c r="G22">
+        <v>3925</v>
+      </c>
+      <c r="H22">
         <v>48</v>
       </c>
-      <c r="C22">
-        <v>125764</v>
-      </c>
-      <c r="D22">
-        <v>19765</v>
-      </c>
-      <c r="E22">
-        <v>216</v>
-      </c>
-      <c r="F22">
-        <v>421</v>
-      </c>
-      <c r="G22">
-        <v>4081</v>
-      </c>
-      <c r="H22">
-        <v>34</v>
-      </c>
       <c r="I22">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="J22">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="K22">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C23">
-        <v>140186</v>
+        <v>125764</v>
       </c>
       <c r="D23">
-        <v>29063</v>
+        <v>19765</v>
       </c>
       <c r="E23">
-        <v>681</v>
+        <v>216</v>
       </c>
       <c r="F23">
-        <v>208</v>
+        <v>421</v>
       </c>
       <c r="G23">
-        <v>2482</v>
+        <v>4081</v>
       </c>
       <c r="H23">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="I23">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="J23">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="K23">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>15</v>
       </c>
       <c r="B24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24">
+        <v>140186</v>
+      </c>
+      <c r="D24">
+        <v>29063</v>
+      </c>
+      <c r="E24">
+        <v>681</v>
+      </c>
+      <c r="F24">
+        <v>208</v>
+      </c>
+      <c r="G24">
+        <v>2482</v>
+      </c>
+      <c r="H24">
+        <v>30</v>
+      </c>
+      <c r="I24">
+        <v>13</v>
+      </c>
+      <c r="J24">
+        <v>62</v>
+      </c>
+      <c r="K24">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" t="s">
         <v>50</v>
       </c>
-      <c r="C24">
+      <c r="C25">
         <v>494577</v>
       </c>
-      <c r="D24">
+      <c r="D25">
         <v>103599</v>
       </c>
-      <c r="E24">
+      <c r="E25">
         <v>2517</v>
       </c>
-      <c r="F24">
+      <c r="F25">
         <v>3831</v>
       </c>
-      <c r="G24">
+      <c r="G25">
         <v>42205</v>
       </c>
-      <c r="H24">
+      <c r="H25">
         <v>555</v>
       </c>
-      <c r="I24">
+      <c r="I25">
         <v>208</v>
       </c>
-      <c r="J24">
+      <c r="J25">
         <v>385</v>
       </c>
-      <c r="K24">
+      <c r="K25">
         <v>1182</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
-      <c r="A25" t="s">
-        <v>16</v>
-      </c>
-      <c r="B25" t="s">
-        <v>51</v>
-      </c>
-      <c r="C25">
-        <v>4100</v>
-      </c>
-      <c r="D25">
-        <v>178</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="F25">
-        <v>235</v>
-      </c>
-      <c r="G25">
-        <v>148</v>
-      </c>
-      <c r="H25">
-        <v>0</v>
-      </c>
-      <c r="I25">
-        <v>0</v>
-      </c>
-      <c r="J25">
-        <v>0</v>
-      </c>
-      <c r="K25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C26">
-        <v>192331</v>
+        <v>4100</v>
       </c>
       <c r="D26">
-        <v>50659</v>
+        <v>178</v>
       </c>
       <c r="E26">
-        <v>417</v>
+        <v>0</v>
       </c>
       <c r="F26">
-        <v>2998</v>
+        <v>235</v>
       </c>
       <c r="G26">
-        <v>20077</v>
+        <v>148</v>
       </c>
       <c r="H26">
-        <v>203</v>
+        <v>0</v>
       </c>
       <c r="I26">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="J26">
-        <v>117</v>
+        <v>0</v>
       </c>
       <c r="K26">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C27">
-        <v>287114</v>
+        <v>192331</v>
       </c>
       <c r="D27">
-        <v>55244</v>
+        <v>50659</v>
       </c>
       <c r="E27">
-        <v>946</v>
+        <v>417</v>
       </c>
       <c r="F27">
-        <v>1623</v>
+        <v>2998</v>
       </c>
       <c r="G27">
-        <v>17294</v>
+        <v>20077</v>
       </c>
       <c r="H27">
-        <v>224</v>
+        <v>203</v>
       </c>
       <c r="I27">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="J27">
-        <v>221</v>
+        <v>117</v>
       </c>
       <c r="K27">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C28">
-        <v>74072</v>
+        <v>287114</v>
       </c>
       <c r="D28">
-        <v>28255</v>
+        <v>55244</v>
       </c>
       <c r="E28">
-        <v>209</v>
+        <v>946</v>
       </c>
       <c r="F28">
-        <v>192</v>
+        <v>1623</v>
       </c>
       <c r="G28">
-        <v>5399</v>
+        <v>17294</v>
       </c>
       <c r="H28">
-        <v>48</v>
+        <v>224</v>
       </c>
       <c r="I28">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="J28">
-        <v>37</v>
+        <v>221</v>
       </c>
       <c r="K28">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>16</v>
       </c>
       <c r="B29" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29">
+        <v>74072</v>
+      </c>
+      <c r="D29">
+        <v>28255</v>
+      </c>
+      <c r="E29">
+        <v>209</v>
+      </c>
+      <c r="F29">
+        <v>192</v>
+      </c>
+      <c r="G29">
+        <v>5399</v>
+      </c>
+      <c r="H29">
+        <v>48</v>
+      </c>
+      <c r="I29">
+        <v>7</v>
+      </c>
+      <c r="J29">
+        <v>37</v>
+      </c>
+      <c r="K29">
         <v>55</v>
       </c>
-      <c r="C29">
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30">
         <v>28314</v>
       </c>
-      <c r="D29">
+      <c r="D30">
         <v>12561</v>
       </c>
-      <c r="E29">
+      <c r="E30">
         <v>65</v>
       </c>
-      <c r="F29">
+      <c r="F30">
         <v>101</v>
       </c>
-      <c r="G29">
+      <c r="G30">
         <v>1971</v>
       </c>
-      <c r="H29">
+      <c r="H30">
         <v>14</v>
       </c>
-      <c r="I29">
+      <c r="I30">
         <v>4</v>
       </c>
-      <c r="J29">
+      <c r="J30">
         <v>19</v>
       </c>
-      <c r="K29">
+      <c r="K30">
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
-      <c r="A30" t="s">
-        <v>17</v>
-      </c>
-      <c r="B30" t="s">
-        <v>56</v>
-      </c>
-      <c r="C30">
-        <v>29420</v>
-      </c>
-      <c r="D30">
-        <v>13471</v>
-      </c>
-      <c r="E30">
-        <v>95</v>
-      </c>
-      <c r="F30">
-        <v>288</v>
-      </c>
-      <c r="G30">
-        <v>5195</v>
-      </c>
-      <c r="H30">
-        <v>44</v>
-      </c>
-      <c r="I30">
-        <v>14</v>
-      </c>
-      <c r="J30">
-        <v>153</v>
-      </c>
-      <c r="K30">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>17</v>
       </c>
       <c r="B31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C31">
-        <v>148464</v>
+        <v>29420</v>
       </c>
       <c r="D31">
-        <v>12056</v>
+        <v>13471</v>
       </c>
       <c r="E31">
-        <v>453</v>
+        <v>95</v>
       </c>
       <c r="F31">
-        <v>1195</v>
+        <v>288</v>
       </c>
       <c r="G31">
-        <v>6709</v>
+        <v>5195</v>
       </c>
       <c r="H31">
-        <v>138</v>
+        <v>44</v>
       </c>
       <c r="I31">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="J31">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="K31">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>17</v>
       </c>
       <c r="B32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C32">
-        <v>672690</v>
+        <v>148464</v>
       </c>
       <c r="D32">
-        <v>50452</v>
+        <v>12056</v>
       </c>
       <c r="E32">
-        <v>1466</v>
+        <v>453</v>
       </c>
       <c r="F32">
-        <v>1546</v>
+        <v>1195</v>
       </c>
       <c r="G32">
-        <v>10380</v>
+        <v>6709</v>
       </c>
       <c r="H32">
-        <v>175</v>
+        <v>138</v>
       </c>
       <c r="I32">
-        <v>299</v>
+        <v>50</v>
       </c>
       <c r="J32">
-        <v>785</v>
+        <v>159</v>
       </c>
       <c r="K32">
-        <v>1410</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>17</v>
       </c>
       <c r="B33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C33">
-        <v>392331</v>
+        <v>672690</v>
       </c>
       <c r="D33">
-        <v>56929</v>
+        <v>50452</v>
       </c>
       <c r="E33">
-        <v>1032</v>
+        <v>1466</v>
       </c>
       <c r="F33">
-        <v>2707</v>
+        <v>1546</v>
       </c>
       <c r="G33">
-        <v>31241</v>
+        <v>10380</v>
       </c>
       <c r="H33">
-        <v>223</v>
+        <v>175</v>
       </c>
       <c r="I33">
-        <v>118</v>
+        <v>299</v>
       </c>
       <c r="J33">
-        <v>624</v>
+        <v>785</v>
       </c>
       <c r="K33">
-        <v>1022</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>17</v>
       </c>
       <c r="B34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C34">
-        <v>515702</v>
+        <v>392331</v>
       </c>
       <c r="D34">
-        <v>27663</v>
+        <v>56929</v>
       </c>
       <c r="E34">
-        <v>497</v>
+        <v>1032</v>
       </c>
       <c r="F34">
-        <v>2412</v>
+        <v>2707</v>
       </c>
       <c r="G34">
-        <v>12417</v>
+        <v>31241</v>
       </c>
       <c r="H34">
-        <v>65</v>
+        <v>223</v>
       </c>
       <c r="I34">
-        <v>141</v>
+        <v>118</v>
       </c>
       <c r="J34">
-        <v>296</v>
+        <v>624</v>
       </c>
       <c r="K34">
-        <v>967</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>17</v>
       </c>
       <c r="B35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C35">
-        <v>260255</v>
+        <v>515702</v>
       </c>
       <c r="D35">
-        <v>28880</v>
+        <v>27663</v>
       </c>
       <c r="E35">
-        <v>594</v>
+        <v>497</v>
       </c>
       <c r="F35">
-        <v>1351</v>
+        <v>2412</v>
       </c>
       <c r="G35">
-        <v>12940</v>
+        <v>12417</v>
       </c>
       <c r="H35">
-        <v>116</v>
+        <v>65</v>
       </c>
       <c r="I35">
-        <v>64</v>
+        <v>141</v>
       </c>
       <c r="J35">
-        <v>173</v>
+        <v>296</v>
       </c>
       <c r="K35">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>17</v>
       </c>
       <c r="B36" t="s">
+        <v>61</v>
+      </c>
+      <c r="C36">
+        <v>260255</v>
+      </c>
+      <c r="D36">
+        <v>28880</v>
+      </c>
+      <c r="E36">
+        <v>594</v>
+      </c>
+      <c r="F36">
+        <v>1351</v>
+      </c>
+      <c r="G36">
+        <v>12940</v>
+      </c>
+      <c r="H36">
+        <v>116</v>
+      </c>
+      <c r="I36">
+        <v>64</v>
+      </c>
+      <c r="J36">
+        <v>173</v>
+      </c>
+      <c r="K36">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" t="s">
         <v>62</v>
       </c>
-      <c r="C36">
+      <c r="C37">
         <v>162177</v>
       </c>
-      <c r="D36">
+      <c r="D37">
         <v>15366</v>
       </c>
-      <c r="E36">
+      <c r="E37">
         <v>521</v>
       </c>
-      <c r="F36">
+      <c r="F37">
         <v>1282</v>
       </c>
-      <c r="G36">
+      <c r="G37">
         <v>13819</v>
       </c>
-      <c r="H36">
+      <c r="H37">
         <v>205</v>
       </c>
-      <c r="I36">
+      <c r="I37">
         <v>67</v>
       </c>
-      <c r="J36">
+      <c r="J37">
         <v>327</v>
       </c>
-      <c r="K36">
+      <c r="K37">
         <v>527</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
-      <c r="A37" t="s">
-        <v>18</v>
-      </c>
-      <c r="B37" t="s">
-        <v>63</v>
-      </c>
-      <c r="C37">
-        <v>518305</v>
-      </c>
-      <c r="D37">
-        <v>55225</v>
-      </c>
-      <c r="E37">
-        <v>1095</v>
-      </c>
-      <c r="F37">
-        <v>1988</v>
-      </c>
-      <c r="G37">
-        <v>17165</v>
-      </c>
-      <c r="H37">
-        <v>153</v>
-      </c>
-      <c r="I37">
-        <v>189</v>
-      </c>
-      <c r="J37">
-        <v>577</v>
-      </c>
-      <c r="K37">
-        <v>1151</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>18</v>
       </c>
       <c r="B38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C38">
-        <v>757387</v>
+        <v>518305</v>
       </c>
       <c r="D38">
-        <v>75724</v>
+        <v>55225</v>
       </c>
       <c r="E38">
-        <v>2202</v>
+        <v>1095</v>
       </c>
       <c r="F38">
-        <v>1258</v>
+        <v>1988</v>
       </c>
       <c r="G38">
-        <v>8156</v>
+        <v>17165</v>
       </c>
       <c r="H38">
-        <v>223</v>
+        <v>153</v>
       </c>
       <c r="I38">
-        <v>442</v>
+        <v>189</v>
       </c>
       <c r="J38">
-        <v>1127</v>
+        <v>577</v>
       </c>
       <c r="K38">
-        <v>2306</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>18</v>
       </c>
       <c r="B39" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C39">
-        <v>646634</v>
+        <v>757387</v>
       </c>
       <c r="D39">
-        <v>69810</v>
+        <v>75724</v>
       </c>
       <c r="E39">
-        <v>1481</v>
+        <v>2202</v>
       </c>
       <c r="F39">
-        <v>901</v>
+        <v>1258</v>
       </c>
       <c r="G39">
-        <v>7406</v>
+        <v>8156</v>
       </c>
       <c r="H39">
-        <v>128</v>
+        <v>223</v>
       </c>
       <c r="I39">
-        <v>315</v>
+        <v>442</v>
       </c>
       <c r="J39">
-        <v>1019</v>
+        <v>1127</v>
       </c>
       <c r="K39">
-        <v>1357</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11">
+        <v>2306</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>18</v>
       </c>
       <c r="B40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C40">
-        <v>287040</v>
+        <v>646634</v>
       </c>
       <c r="D40">
-        <v>93166</v>
+        <v>69810</v>
       </c>
       <c r="E40">
-        <v>1733</v>
+        <v>1481</v>
       </c>
       <c r="F40">
-        <v>6606</v>
+        <v>901</v>
       </c>
       <c r="G40">
-        <v>81607</v>
+        <v>7406</v>
       </c>
       <c r="H40">
-        <v>1128</v>
+        <v>128</v>
       </c>
       <c r="I40">
-        <v>171</v>
+        <v>315</v>
       </c>
       <c r="J40">
-        <v>646</v>
+        <v>1019</v>
       </c>
       <c r="K40">
-        <v>1139</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11">
+        <v>1357</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>18</v>
       </c>
       <c r="B41" t="s">
+        <v>66</v>
+      </c>
+      <c r="C41">
+        <v>287040</v>
+      </c>
+      <c r="D41">
+        <v>93166</v>
+      </c>
+      <c r="E41">
+        <v>1733</v>
+      </c>
+      <c r="F41">
+        <v>6606</v>
+      </c>
+      <c r="G41">
+        <v>81607</v>
+      </c>
+      <c r="H41">
+        <v>1128</v>
+      </c>
+      <c r="I41">
+        <v>171</v>
+      </c>
+      <c r="J41">
+        <v>646</v>
+      </c>
+      <c r="K41">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>18</v>
+      </c>
+      <c r="B42" t="s">
         <v>67</v>
       </c>
-      <c r="C41">
+      <c r="C42">
         <v>544853</v>
       </c>
-      <c r="D41">
+      <c r="D42">
         <v>77502</v>
       </c>
-      <c r="E41">
+      <c r="E42">
         <v>2275</v>
       </c>
-      <c r="F41">
+      <c r="F42">
         <v>1089</v>
       </c>
-      <c r="G41">
+      <c r="G42">
         <v>8570</v>
       </c>
-      <c r="H41">
+      <c r="H42">
         <v>304</v>
       </c>
-      <c r="I41">
+      <c r="I42">
         <v>258</v>
       </c>
-      <c r="J41">
+      <c r="J42">
         <v>916</v>
       </c>
-      <c r="K41">
+      <c r="K42">
         <v>1407</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
-      <c r="A42" t="s">
-        <v>19</v>
-      </c>
-      <c r="B42" t="s">
-        <v>68</v>
-      </c>
-      <c r="C42">
-        <v>8085</v>
-      </c>
-      <c r="D42">
-        <v>8158</v>
-      </c>
-      <c r="E42">
-        <v>11</v>
-      </c>
-      <c r="F42">
-        <v>72</v>
-      </c>
-      <c r="G42">
-        <v>3732</v>
-      </c>
-      <c r="H42">
-        <v>14</v>
-      </c>
-      <c r="I42">
-        <v>0</v>
-      </c>
-      <c r="J42">
-        <v>5</v>
-      </c>
-      <c r="K42">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>19</v>
       </c>
       <c r="B43" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C43">
-        <v>61627</v>
+        <v>8085</v>
       </c>
       <c r="D43">
-        <v>76640</v>
+        <v>8158</v>
       </c>
       <c r="E43">
-        <v>192</v>
+        <v>11</v>
       </c>
       <c r="F43">
-        <v>2645</v>
+        <v>72</v>
       </c>
       <c r="G43">
-        <v>80318</v>
+        <v>3732</v>
       </c>
       <c r="H43">
-        <v>286</v>
+        <v>14</v>
       </c>
       <c r="I43">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="J43">
-        <v>219</v>
+        <v>5</v>
       </c>
       <c r="K43">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>19</v>
       </c>
       <c r="B44" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C44">
-        <v>142495</v>
+        <v>61627</v>
       </c>
       <c r="D44">
-        <v>162405</v>
+        <v>76640</v>
       </c>
       <c r="E44">
-        <v>336</v>
+        <v>192</v>
       </c>
       <c r="F44">
-        <v>1711</v>
+        <v>2645</v>
       </c>
       <c r="G44">
-        <v>89250</v>
+        <v>80318</v>
       </c>
       <c r="H44">
-        <v>245</v>
+        <v>286</v>
       </c>
       <c r="I44">
-        <v>76</v>
+        <v>15</v>
       </c>
       <c r="J44">
-        <v>421</v>
+        <v>219</v>
       </c>
       <c r="K44">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>19</v>
       </c>
       <c r="B45" t="s">
+        <v>70</v>
+      </c>
+      <c r="C45">
+        <v>142495</v>
+      </c>
+      <c r="D45">
+        <v>162405</v>
+      </c>
+      <c r="E45">
+        <v>336</v>
+      </c>
+      <c r="F45">
+        <v>1711</v>
+      </c>
+      <c r="G45">
+        <v>89250</v>
+      </c>
+      <c r="H45">
+        <v>245</v>
+      </c>
+      <c r="I45">
+        <v>76</v>
+      </c>
+      <c r="J45">
+        <v>421</v>
+      </c>
+      <c r="K45">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>19</v>
+      </c>
+      <c r="B46" t="s">
         <v>71</v>
       </c>
-      <c r="C45">
+      <c r="C46">
         <v>31104</v>
       </c>
-      <c r="D45">
+      <c r="D46">
         <v>43268</v>
       </c>
-      <c r="E45">
+      <c r="E46">
         <v>46</v>
       </c>
-      <c r="F45">
+      <c r="F46">
         <v>1351</v>
       </c>
-      <c r="G45">
+      <c r="G46">
         <v>61907</v>
       </c>
-      <c r="H45">
+      <c r="H46">
         <v>121</v>
       </c>
-      <c r="I45">
+      <c r="I46">
         <v>31</v>
       </c>
-      <c r="J45">
+      <c r="J46">
         <v>71</v>
       </c>
-      <c r="K45">
+      <c r="K46">
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="1:11">
-      <c r="A46" t="s">
-        <v>20</v>
-      </c>
-      <c r="B46" t="s">
-        <v>72</v>
-      </c>
-      <c r="C46">
-        <v>171126</v>
-      </c>
-      <c r="D46">
-        <v>20550</v>
-      </c>
-      <c r="E46">
-        <v>451</v>
-      </c>
-      <c r="F46">
-        <v>20539</v>
-      </c>
-      <c r="G46">
-        <v>60428</v>
-      </c>
-      <c r="H46">
-        <v>643</v>
-      </c>
-      <c r="I46">
-        <v>310</v>
-      </c>
-      <c r="J46">
-        <v>437</v>
-      </c>
-      <c r="K46">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>20</v>
       </c>
       <c r="B47" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C47">
-        <v>69598</v>
+        <v>171126</v>
       </c>
       <c r="D47">
-        <v>12420</v>
+        <v>20550</v>
       </c>
       <c r="E47">
-        <v>89</v>
+        <v>451</v>
       </c>
       <c r="F47">
-        <v>9520</v>
+        <v>20539</v>
       </c>
       <c r="G47">
-        <v>36200</v>
+        <v>60428</v>
       </c>
       <c r="H47">
-        <v>227</v>
+        <v>643</v>
       </c>
       <c r="I47">
-        <v>26</v>
+        <v>310</v>
       </c>
       <c r="J47">
-        <v>94</v>
+        <v>437</v>
       </c>
       <c r="K47">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>20</v>
       </c>
       <c r="B48" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C48">
-        <v>207047</v>
+        <v>69598</v>
       </c>
       <c r="D48">
-        <v>45747</v>
+        <v>12420</v>
       </c>
       <c r="E48">
-        <v>496</v>
+        <v>89</v>
       </c>
       <c r="F48">
-        <v>19535</v>
+        <v>9520</v>
       </c>
       <c r="G48">
-        <v>119552</v>
+        <v>36200</v>
       </c>
       <c r="H48">
-        <v>828</v>
+        <v>227</v>
       </c>
       <c r="I48">
-        <v>141</v>
+        <v>26</v>
       </c>
       <c r="J48">
-        <v>401</v>
+        <v>94</v>
       </c>
       <c r="K48">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>20</v>
       </c>
       <c r="B49" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C49">
-        <v>28518</v>
+        <v>207047</v>
       </c>
       <c r="D49">
-        <v>8514</v>
+        <v>45747</v>
       </c>
       <c r="E49">
-        <v>128</v>
+        <v>496</v>
       </c>
       <c r="F49">
-        <v>2359</v>
+        <v>19535</v>
       </c>
       <c r="G49">
-        <v>13123</v>
+        <v>119552</v>
       </c>
       <c r="H49">
-        <v>221</v>
+        <v>828</v>
       </c>
       <c r="I49">
-        <v>29</v>
+        <v>141</v>
       </c>
       <c r="J49">
-        <v>86</v>
+        <v>401</v>
       </c>
       <c r="K49">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>20</v>
       </c>
       <c r="B50" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C50">
-        <v>62075</v>
+        <v>28518</v>
       </c>
       <c r="D50">
-        <v>45847</v>
+        <v>8514</v>
       </c>
       <c r="E50">
-        <v>384</v>
+        <v>128</v>
       </c>
       <c r="F50">
-        <v>4606</v>
+        <v>2359</v>
       </c>
       <c r="G50">
-        <v>70612</v>
+        <v>13123</v>
       </c>
       <c r="H50">
-        <v>427</v>
+        <v>221</v>
       </c>
       <c r="I50">
-        <v>68</v>
+        <v>29</v>
       </c>
       <c r="J50">
-        <v>360</v>
+        <v>86</v>
       </c>
       <c r="K50">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>20</v>
       </c>
       <c r="B51" t="s">
+        <v>76</v>
+      </c>
+      <c r="C51">
+        <v>62075</v>
+      </c>
+      <c r="D51">
+        <v>45847</v>
+      </c>
+      <c r="E51">
+        <v>384</v>
+      </c>
+      <c r="F51">
+        <v>4606</v>
+      </c>
+      <c r="G51">
+        <v>70612</v>
+      </c>
+      <c r="H51">
+        <v>427</v>
+      </c>
+      <c r="I51">
+        <v>68</v>
+      </c>
+      <c r="J51">
+        <v>360</v>
+      </c>
+      <c r="K51">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>20</v>
+      </c>
+      <c r="B52" t="s">
         <v>77</v>
       </c>
-      <c r="C51">
+      <c r="C52">
         <v>78005</v>
       </c>
-      <c r="D51">
+      <c r="D52">
         <v>10986</v>
       </c>
-      <c r="E51">
+      <c r="E52">
         <v>156</v>
       </c>
-      <c r="F51">
+      <c r="F52">
         <v>22385</v>
       </c>
-      <c r="G51">
+      <c r="G52">
         <v>53292</v>
       </c>
-      <c r="H51">
+      <c r="H52">
         <v>347</v>
       </c>
-      <c r="I51">
+      <c r="I52">
         <v>43</v>
       </c>
-      <c r="J51">
+      <c r="J52">
         <v>82</v>
       </c>
-      <c r="K51">
+      <c r="K52">
         <v>120</v>
       </c>
     </row>
-    <row r="52" spans="1:11">
-      <c r="A52" t="s">
-        <v>21</v>
-      </c>
-      <c r="B52" t="s">
-        <v>78</v>
-      </c>
-      <c r="C52">
-        <v>67244</v>
-      </c>
-      <c r="D52">
-        <v>25100</v>
-      </c>
-      <c r="E52">
-        <v>221</v>
-      </c>
-      <c r="F52">
-        <v>6128</v>
-      </c>
-      <c r="G52">
-        <v>33013</v>
-      </c>
-      <c r="H52">
-        <v>199</v>
-      </c>
-      <c r="I52">
-        <v>206</v>
-      </c>
-      <c r="J52">
-        <v>196</v>
-      </c>
-      <c r="K52">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>21</v>
       </c>
       <c r="B53" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C53">
-        <v>59377</v>
+        <v>67244</v>
       </c>
       <c r="D53">
-        <v>44827</v>
+        <v>25100</v>
       </c>
       <c r="E53">
-        <v>290</v>
+        <v>221</v>
       </c>
       <c r="F53">
-        <v>1603</v>
+        <v>6128</v>
       </c>
       <c r="G53">
-        <v>21383</v>
+        <v>33013</v>
       </c>
       <c r="H53">
-        <v>105</v>
+        <v>199</v>
       </c>
       <c r="I53">
-        <v>19</v>
+        <v>206</v>
       </c>
       <c r="J53">
-        <v>81</v>
+        <v>196</v>
       </c>
       <c r="K53">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>21</v>
       </c>
       <c r="B54" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C54">
-        <v>83383</v>
+        <v>59377</v>
       </c>
       <c r="D54">
-        <v>75679</v>
+        <v>44827</v>
       </c>
       <c r="E54">
-        <v>1255</v>
+        <v>290</v>
       </c>
       <c r="F54">
-        <v>868</v>
+        <v>1603</v>
       </c>
       <c r="G54">
-        <v>15208</v>
+        <v>21383</v>
       </c>
       <c r="H54">
-        <v>227</v>
+        <v>105</v>
       </c>
       <c r="I54">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="J54">
-        <v>233</v>
+        <v>81</v>
       </c>
       <c r="K54">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>21</v>
       </c>
       <c r="B55" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C55">
-        <v>18828</v>
+        <v>83383</v>
       </c>
       <c r="D55">
-        <v>15377</v>
+        <v>75679</v>
       </c>
       <c r="E55">
-        <v>64</v>
+        <v>1255</v>
       </c>
       <c r="F55">
-        <v>210</v>
+        <v>868</v>
       </c>
       <c r="G55">
-        <v>5740</v>
+        <v>15208</v>
       </c>
       <c r="H55">
-        <v>33</v>
+        <v>227</v>
       </c>
       <c r="I55">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="J55">
-        <v>30</v>
+        <v>233</v>
       </c>
       <c r="K55">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>21</v>
       </c>
       <c r="B56" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C56">
-        <v>260543</v>
+        <v>18828</v>
       </c>
       <c r="D56">
-        <v>212528</v>
+        <v>15377</v>
       </c>
       <c r="E56">
-        <v>2679</v>
+        <v>64</v>
       </c>
       <c r="F56">
-        <v>2104</v>
+        <v>210</v>
       </c>
       <c r="G56">
-        <v>38840</v>
+        <v>5740</v>
       </c>
       <c r="H56">
-        <v>498</v>
+        <v>33</v>
       </c>
       <c r="I56">
-        <v>164</v>
+        <v>6</v>
       </c>
       <c r="J56">
-        <v>682</v>
+        <v>30</v>
       </c>
       <c r="K56">
-        <v>1359</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>21</v>
       </c>
       <c r="B57" t="s">
+        <v>82</v>
+      </c>
+      <c r="C57">
+        <v>260543</v>
+      </c>
+      <c r="D57">
+        <v>212528</v>
+      </c>
+      <c r="E57">
+        <v>2679</v>
+      </c>
+      <c r="F57">
+        <v>2104</v>
+      </c>
+      <c r="G57">
+        <v>38840</v>
+      </c>
+      <c r="H57">
+        <v>498</v>
+      </c>
+      <c r="I57">
+        <v>164</v>
+      </c>
+      <c r="J57">
+        <v>682</v>
+      </c>
+      <c r="K57">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>21</v>
+      </c>
+      <c r="B58" t="s">
         <v>83</v>
       </c>
-      <c r="C57">
+      <c r="C58">
         <v>342557</v>
       </c>
-      <c r="D57">
+      <c r="D58">
         <v>224274</v>
       </c>
-      <c r="E57">
+      <c r="E58">
         <v>2826</v>
       </c>
-      <c r="F57">
+      <c r="F58">
         <v>5437</v>
       </c>
-      <c r="G57">
+      <c r="G58">
         <v>106669</v>
       </c>
-      <c r="H57">
+      <c r="H58">
         <v>720</v>
       </c>
-      <c r="I57">
+      <c r="I58">
         <v>215</v>
       </c>
-      <c r="J57">
+      <c r="J58">
         <v>848</v>
       </c>
-      <c r="K57">
+      <c r="K58">
         <v>1704</v>
       </c>
     </row>
-    <row r="58" spans="1:11">
-      <c r="A58" t="s">
-        <v>22</v>
-      </c>
-      <c r="B58" t="s">
-        <v>84</v>
-      </c>
-      <c r="C58">
-        <v>163992</v>
-      </c>
-      <c r="D58">
-        <v>88748</v>
-      </c>
-      <c r="E58">
-        <v>747</v>
-      </c>
-      <c r="F58">
-        <v>1625</v>
-      </c>
-      <c r="G58">
-        <v>29818</v>
-      </c>
-      <c r="H58">
-        <v>233</v>
-      </c>
-      <c r="I58">
-        <v>46</v>
-      </c>
-      <c r="J58">
-        <v>183</v>
-      </c>
-      <c r="K58">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>22</v>
       </c>
       <c r="B59" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C59">
-        <v>640393</v>
+        <v>163992</v>
       </c>
       <c r="D59">
-        <v>347331</v>
+        <v>88748</v>
       </c>
       <c r="E59">
-        <v>5476</v>
+        <v>747</v>
       </c>
       <c r="F59">
-        <v>2689</v>
+        <v>1625</v>
       </c>
       <c r="G59">
-        <v>49413</v>
+        <v>29818</v>
       </c>
       <c r="H59">
-        <v>977</v>
+        <v>233</v>
       </c>
       <c r="I59">
-        <v>341</v>
+        <v>46</v>
       </c>
       <c r="J59">
-        <v>1862</v>
+        <v>183</v>
       </c>
       <c r="K59">
-        <v>2577</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>22</v>
       </c>
       <c r="B60" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C60">
-        <v>120763</v>
+        <v>640393</v>
       </c>
       <c r="D60">
-        <v>95080</v>
+        <v>347331</v>
       </c>
       <c r="E60">
-        <v>892</v>
+        <v>5476</v>
       </c>
       <c r="F60">
-        <v>5862</v>
+        <v>2689</v>
       </c>
       <c r="G60">
-        <v>81706</v>
+        <v>49413</v>
       </c>
       <c r="H60">
-        <v>475</v>
+        <v>977</v>
       </c>
       <c r="I60">
-        <v>62</v>
+        <v>341</v>
       </c>
       <c r="J60">
-        <v>388</v>
+        <v>1862</v>
       </c>
       <c r="K60">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11">
+        <v>2577</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>22</v>
       </c>
       <c r="B61" t="s">
+        <v>86</v>
+      </c>
+      <c r="C61">
+        <v>120763</v>
+      </c>
+      <c r="D61">
+        <v>95080</v>
+      </c>
+      <c r="E61">
+        <v>892</v>
+      </c>
+      <c r="F61">
+        <v>5862</v>
+      </c>
+      <c r="G61">
+        <v>81706</v>
+      </c>
+      <c r="H61">
+        <v>475</v>
+      </c>
+      <c r="I61">
+        <v>62</v>
+      </c>
+      <c r="J61">
+        <v>388</v>
+      </c>
+      <c r="K61">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>22</v>
+      </c>
+      <c r="B62" t="s">
         <v>87</v>
       </c>
-      <c r="C61">
+      <c r="C62">
         <v>12399</v>
       </c>
-      <c r="D61">
+      <c r="D62">
         <v>7905</v>
       </c>
-      <c r="E61">
+      <c r="E62">
         <v>56</v>
       </c>
-      <c r="F61">
+      <c r="F62">
         <v>168</v>
       </c>
-      <c r="G61">
+      <c r="G62">
         <v>1984</v>
       </c>
-      <c r="H61">
+      <c r="H62">
         <v>18</v>
       </c>
-      <c r="I61">
+      <c r="I62">
         <v>2</v>
       </c>
-      <c r="J61">
+      <c r="J62">
         <v>4</v>
       </c>
-      <c r="K61">
+      <c r="K62">
         <v>17</v>
       </c>
     </row>
-    <row r="62" spans="1:11">
-      <c r="A62" t="s">
-        <v>23</v>
-      </c>
-      <c r="B62" t="s">
-        <v>88</v>
-      </c>
-      <c r="C62">
-        <v>20253</v>
-      </c>
-      <c r="D62">
-        <v>12537</v>
-      </c>
-      <c r="E62">
-        <v>228</v>
-      </c>
-      <c r="F62">
-        <v>347</v>
-      </c>
-      <c r="G62">
-        <v>4433</v>
-      </c>
-      <c r="H62">
-        <v>105</v>
-      </c>
-      <c r="I62">
-        <v>10</v>
-      </c>
-      <c r="J62">
-        <v>35</v>
-      </c>
-      <c r="K62">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>23</v>
       </c>
       <c r="B63" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C63">
-        <v>39223</v>
+        <v>20253</v>
       </c>
       <c r="D63">
-        <v>47819</v>
+        <v>12537</v>
       </c>
       <c r="E63">
-        <v>1253</v>
+        <v>228</v>
       </c>
       <c r="F63">
-        <v>848</v>
+        <v>347</v>
       </c>
       <c r="G63">
-        <v>14736</v>
+        <v>4433</v>
       </c>
       <c r="H63">
-        <v>452</v>
+        <v>105</v>
       </c>
       <c r="I63">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="J63">
-        <v>267</v>
+        <v>35</v>
       </c>
       <c r="K63">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>23</v>
       </c>
       <c r="B64" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C64">
-        <v>211309</v>
+        <v>39223</v>
       </c>
       <c r="D64">
-        <v>188231</v>
+        <v>47819</v>
       </c>
       <c r="E64">
-        <v>8143</v>
+        <v>1253</v>
       </c>
       <c r="F64">
-        <v>2690</v>
+        <v>848</v>
       </c>
       <c r="G64">
-        <v>30665</v>
+        <v>14736</v>
       </c>
       <c r="H64">
-        <v>1764</v>
+        <v>452</v>
       </c>
       <c r="I64">
-        <v>353</v>
+        <v>44</v>
       </c>
       <c r="J64">
-        <v>1503</v>
+        <v>267</v>
       </c>
       <c r="K64">
-        <v>3314</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>23</v>
       </c>
       <c r="B65" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C65">
-        <v>44277</v>
+        <v>211309</v>
       </c>
       <c r="D65">
-        <v>23329</v>
+        <v>188231</v>
       </c>
       <c r="E65">
-        <v>185</v>
+        <v>8143</v>
       </c>
       <c r="F65">
-        <v>5889</v>
+        <v>2690</v>
       </c>
       <c r="G65">
-        <v>50060</v>
+        <v>30665</v>
       </c>
       <c r="H65">
-        <v>356</v>
+        <v>1764</v>
       </c>
       <c r="I65">
-        <v>34</v>
+        <v>353</v>
       </c>
       <c r="J65">
-        <v>193</v>
+        <v>1503</v>
       </c>
       <c r="K65">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11">
+        <v>3314</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>23</v>
       </c>
       <c r="B66" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C66">
-        <v>55643</v>
+        <v>44277</v>
       </c>
       <c r="D66">
-        <v>50874</v>
+        <v>23329</v>
       </c>
       <c r="E66">
-        <v>894</v>
+        <v>185</v>
       </c>
       <c r="F66">
-        <v>2934</v>
+        <v>5889</v>
       </c>
       <c r="G66">
-        <v>50716</v>
+        <v>50060</v>
       </c>
       <c r="H66">
-        <v>551</v>
+        <v>356</v>
       </c>
       <c r="I66">
-        <v>76</v>
+        <v>34</v>
       </c>
       <c r="J66">
-        <v>443</v>
+        <v>193</v>
       </c>
       <c r="K66">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>23</v>
       </c>
       <c r="B67" t="s">
+        <v>92</v>
+      </c>
+      <c r="C67">
+        <v>55643</v>
+      </c>
+      <c r="D67">
+        <v>50874</v>
+      </c>
+      <c r="E67">
+        <v>894</v>
+      </c>
+      <c r="F67">
+        <v>2934</v>
+      </c>
+      <c r="G67">
+        <v>50716</v>
+      </c>
+      <c r="H67">
+        <v>551</v>
+      </c>
+      <c r="I67">
+        <v>76</v>
+      </c>
+      <c r="J67">
+        <v>443</v>
+      </c>
+      <c r="K67">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>23</v>
+      </c>
+      <c r="B68" t="s">
         <v>93</v>
       </c>
-      <c r="C67">
+      <c r="C68">
         <v>54626</v>
       </c>
-      <c r="D67">
+      <c r="D68">
         <v>26983</v>
       </c>
-      <c r="E67">
+      <c r="E68">
         <v>144</v>
       </c>
-      <c r="F67">
+      <c r="F68">
         <v>967</v>
       </c>
-      <c r="G67">
+      <c r="G68">
         <v>9198</v>
       </c>
-      <c r="H67">
+      <c r="H68">
         <v>56</v>
       </c>
-      <c r="I67">
+      <c r="I68">
         <v>24</v>
       </c>
-      <c r="J67">
+      <c r="J68">
         <v>78</v>
       </c>
-      <c r="K67">
+      <c r="K68">
         <v>37</v>
       </c>
     </row>
-    <row r="68" spans="1:11">
-      <c r="A68" t="s">
-        <v>24</v>
-      </c>
-      <c r="B68" t="s">
-        <v>94</v>
-      </c>
-      <c r="C68">
-        <v>126174</v>
-      </c>
-      <c r="D68">
-        <v>158528</v>
-      </c>
-      <c r="E68">
-        <v>628</v>
-      </c>
-      <c r="F68">
-        <v>216</v>
-      </c>
-      <c r="G68">
-        <v>17017</v>
-      </c>
-      <c r="H68">
-        <v>125</v>
-      </c>
-      <c r="I68">
-        <v>17</v>
-      </c>
-      <c r="J68">
-        <v>625</v>
-      </c>
-      <c r="K68">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>24</v>
       </c>
       <c r="B69" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C69">
-        <v>11059</v>
+        <v>126174</v>
       </c>
       <c r="D69">
-        <v>7499</v>
+        <v>158528</v>
       </c>
       <c r="E69">
-        <v>7</v>
+        <v>628</v>
       </c>
       <c r="F69">
-        <v>45</v>
+        <v>216</v>
       </c>
       <c r="G69">
-        <v>1321</v>
+        <v>17017</v>
       </c>
       <c r="H69">
-        <v>3</v>
+        <v>125</v>
       </c>
       <c r="I69">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="J69">
-        <v>9</v>
+        <v>625</v>
       </c>
       <c r="K69">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>24</v>
       </c>
       <c r="B70" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C70">
-        <v>85752</v>
+        <v>11059</v>
       </c>
       <c r="D70">
-        <v>79183</v>
+        <v>7499</v>
       </c>
       <c r="E70">
-        <v>186</v>
+        <v>7</v>
       </c>
       <c r="F70">
-        <v>1784</v>
+        <v>45</v>
       </c>
       <c r="G70">
-        <v>33657</v>
+        <v>1321</v>
       </c>
       <c r="H70">
-        <v>170</v>
+        <v>3</v>
       </c>
       <c r="I70">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="J70">
-        <v>315</v>
+        <v>9</v>
       </c>
       <c r="K70">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>24</v>
       </c>
       <c r="B71" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C71">
-        <v>51946</v>
+        <v>85752</v>
       </c>
       <c r="D71">
-        <v>49659</v>
+        <v>79183</v>
       </c>
       <c r="E71">
-        <v>124</v>
+        <v>186</v>
       </c>
       <c r="F71">
-        <v>1488</v>
+        <v>1784</v>
       </c>
       <c r="G71">
-        <v>29342</v>
+        <v>33657</v>
       </c>
       <c r="H71">
-        <v>107</v>
+        <v>170</v>
       </c>
       <c r="I71">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="J71">
-        <v>100</v>
+        <v>315</v>
       </c>
       <c r="K71">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>24</v>
       </c>
       <c r="B72" t="s">
+        <v>97</v>
+      </c>
+      <c r="C72">
+        <v>51946</v>
+      </c>
+      <c r="D72">
+        <v>49659</v>
+      </c>
+      <c r="E72">
+        <v>124</v>
+      </c>
+      <c r="F72">
+        <v>1488</v>
+      </c>
+      <c r="G72">
+        <v>29342</v>
+      </c>
+      <c r="H72">
+        <v>107</v>
+      </c>
+      <c r="I72">
+        <v>12</v>
+      </c>
+      <c r="J72">
+        <v>100</v>
+      </c>
+      <c r="K72">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>24</v>
+      </c>
+      <c r="B73" t="s">
         <v>98</v>
       </c>
-      <c r="C72">
+      <c r="C73">
         <v>191989</v>
       </c>
-      <c r="D72">
+      <c r="D73">
         <v>129188</v>
       </c>
-      <c r="E72">
+      <c r="E73">
         <v>712</v>
       </c>
-      <c r="F72">
+      <c r="F73">
         <v>810</v>
       </c>
-      <c r="G72">
+      <c r="G73">
         <v>27888</v>
       </c>
-      <c r="H72">
+      <c r="H73">
         <v>207</v>
       </c>
-      <c r="I72">
+      <c r="I73">
         <v>40</v>
       </c>
-      <c r="J72">
+      <c r="J73">
         <v>497</v>
       </c>
-      <c r="K72">
+      <c r="K73">
         <v>362</v>
       </c>
     </row>
-    <row r="73" spans="1:11">
-      <c r="A73" t="s">
-        <v>25</v>
-      </c>
-      <c r="B73" t="s">
-        <v>99</v>
-      </c>
-      <c r="C73">
-        <v>70879</v>
-      </c>
-      <c r="D73">
-        <v>77353</v>
-      </c>
-      <c r="E73">
-        <v>942</v>
-      </c>
-      <c r="F73">
-        <v>524</v>
-      </c>
-      <c r="G73">
-        <v>15090</v>
-      </c>
-      <c r="H73">
-        <v>170</v>
-      </c>
-      <c r="I73">
-        <v>17</v>
-      </c>
-      <c r="J73">
-        <v>273</v>
-      </c>
-      <c r="K73">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>25</v>
       </c>
       <c r="B74" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C74">
-        <v>119122</v>
+        <v>70879</v>
       </c>
       <c r="D74">
-        <v>85140</v>
+        <v>77353</v>
       </c>
       <c r="E74">
-        <v>172</v>
+        <v>942</v>
       </c>
       <c r="F74">
-        <v>631</v>
+        <v>524</v>
       </c>
       <c r="G74">
-        <v>22829</v>
+        <v>15090</v>
       </c>
       <c r="H74">
-        <v>53</v>
+        <v>170</v>
       </c>
       <c r="I74">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="J74">
-        <v>332</v>
+        <v>273</v>
       </c>
       <c r="K74">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>25</v>
       </c>
       <c r="B75" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C75">
-        <v>311968</v>
+        <v>119122</v>
       </c>
       <c r="D75">
-        <v>201101</v>
+        <v>85140</v>
       </c>
       <c r="E75">
-        <v>1120</v>
+        <v>172</v>
       </c>
       <c r="F75">
-        <v>1259</v>
+        <v>631</v>
       </c>
       <c r="G75">
-        <v>33836</v>
+        <v>22829</v>
       </c>
       <c r="H75">
-        <v>219</v>
+        <v>53</v>
       </c>
       <c r="I75">
-        <v>93</v>
+        <v>25</v>
       </c>
       <c r="J75">
-        <v>343</v>
+        <v>332</v>
       </c>
       <c r="K75">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>25</v>
       </c>
       <c r="B76" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C76">
-        <v>12338</v>
+        <v>311968</v>
       </c>
       <c r="D76">
-        <v>12053</v>
+        <v>201101</v>
       </c>
       <c r="E76">
-        <v>23</v>
+        <v>1120</v>
       </c>
       <c r="F76">
-        <v>1677</v>
+        <v>1259</v>
       </c>
       <c r="G76">
-        <v>49713</v>
+        <v>33836</v>
       </c>
       <c r="H76">
-        <v>26</v>
+        <v>219</v>
       </c>
       <c r="I76">
-        <v>13</v>
+        <v>93</v>
       </c>
       <c r="J76">
-        <v>26</v>
+        <v>343</v>
       </c>
       <c r="K76">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>25</v>
       </c>
       <c r="B77" t="s">
+        <v>102</v>
+      </c>
+      <c r="C77">
+        <v>12338</v>
+      </c>
+      <c r="D77">
+        <v>12053</v>
+      </c>
+      <c r="E77">
+        <v>23</v>
+      </c>
+      <c r="F77">
+        <v>1677</v>
+      </c>
+      <c r="G77">
+        <v>49713</v>
+      </c>
+      <c r="H77">
+        <v>26</v>
+      </c>
+      <c r="I77">
+        <v>13</v>
+      </c>
+      <c r="J77">
+        <v>26</v>
+      </c>
+      <c r="K77">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>25</v>
+      </c>
+      <c r="B78" t="s">
         <v>103</v>
       </c>
-      <c r="C77">
+      <c r="C78">
         <v>42420</v>
       </c>
-      <c r="D77">
+      <c r="D78">
         <v>47747</v>
       </c>
-      <c r="E77">
+      <c r="E78">
         <v>326</v>
       </c>
-      <c r="F77">
+      <c r="F78">
         <v>1266</v>
       </c>
-      <c r="G77">
+      <c r="G78">
         <v>33070</v>
       </c>
-      <c r="H77">
+      <c r="H78">
         <v>128</v>
       </c>
-      <c r="I77">
+      <c r="I78">
         <v>55</v>
       </c>
-      <c r="J77">
+      <c r="J78">
         <v>313</v>
       </c>
-      <c r="K77">
+      <c r="K78">
         <v>228</v>
       </c>
     </row>
-    <row r="78" spans="1:11">
-      <c r="A78" t="s">
-        <v>26</v>
-      </c>
-      <c r="B78" t="s">
-        <v>104</v>
-      </c>
-      <c r="C78">
-        <v>119647</v>
-      </c>
-      <c r="D78">
-        <v>137125</v>
-      </c>
-      <c r="E78">
-        <v>451</v>
-      </c>
-      <c r="F78">
-        <v>1461</v>
-      </c>
-      <c r="G78">
-        <v>54150</v>
-      </c>
-      <c r="H78">
-        <v>700</v>
-      </c>
-      <c r="I78">
-        <v>20</v>
-      </c>
-      <c r="J78">
-        <v>231</v>
-      </c>
-      <c r="K78">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>26</v>
       </c>
       <c r="B79" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C79">
-        <v>25894</v>
+        <v>119647</v>
       </c>
       <c r="D79">
-        <v>22730</v>
+        <v>137125</v>
       </c>
       <c r="E79">
-        <v>68</v>
+        <v>451</v>
       </c>
       <c r="F79">
-        <v>200</v>
+        <v>1461</v>
       </c>
       <c r="G79">
-        <v>6359</v>
+        <v>54150</v>
       </c>
       <c r="H79">
-        <v>24</v>
+        <v>700</v>
       </c>
       <c r="I79">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="J79">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="K79">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>26</v>
       </c>
       <c r="B80" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C80">
-        <v>33657</v>
+        <v>25894</v>
       </c>
       <c r="D80">
-        <v>41561</v>
+        <v>22730</v>
       </c>
       <c r="E80">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F80">
-        <v>903</v>
+        <v>200</v>
       </c>
       <c r="G80">
-        <v>45874</v>
+        <v>6359</v>
       </c>
       <c r="H80">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="I80">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J80">
-        <v>41</v>
+        <v>236</v>
       </c>
       <c r="K80">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>26</v>
       </c>
       <c r="B81" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C81">
-        <v>200538</v>
+        <v>33657</v>
       </c>
       <c r="D81">
-        <v>114199</v>
+        <v>41561</v>
       </c>
       <c r="E81">
-        <v>448</v>
+        <v>72</v>
       </c>
       <c r="F81">
-        <v>1186</v>
+        <v>903</v>
       </c>
       <c r="G81">
-        <v>38368</v>
+        <v>45874</v>
       </c>
       <c r="H81">
-        <v>135</v>
+        <v>48</v>
       </c>
       <c r="I81">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="J81">
-        <v>260</v>
+        <v>41</v>
       </c>
       <c r="K81">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>26</v>
       </c>
       <c r="B82" t="s">
+        <v>107</v>
+      </c>
+      <c r="C82">
+        <v>200538</v>
+      </c>
+      <c r="D82">
+        <v>114199</v>
+      </c>
+      <c r="E82">
+        <v>448</v>
+      </c>
+      <c r="F82">
+        <v>1186</v>
+      </c>
+      <c r="G82">
+        <v>38368</v>
+      </c>
+      <c r="H82">
+        <v>135</v>
+      </c>
+      <c r="I82">
+        <v>24</v>
+      </c>
+      <c r="J82">
+        <v>260</v>
+      </c>
+      <c r="K82">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>26</v>
+      </c>
+      <c r="B83" t="s">
         <v>108</v>
       </c>
-      <c r="C82">
+      <c r="C83">
         <v>67175</v>
       </c>
-      <c r="D82">
+      <c r="D83">
         <v>57999</v>
       </c>
-      <c r="E82">
+      <c r="E83">
         <v>105</v>
       </c>
-      <c r="F82">
+      <c r="F83">
         <v>1093</v>
       </c>
-      <c r="G82">
+      <c r="G83">
         <v>54916</v>
       </c>
-      <c r="H82">
+      <c r="H83">
         <v>93</v>
       </c>
-      <c r="I82">
+      <c r="I83">
         <v>8</v>
       </c>
-      <c r="J82">
+      <c r="J83">
         <v>111</v>
       </c>
-      <c r="K82">
+      <c r="K83">
         <v>84</v>
       </c>
     </row>
-    <row r="83" spans="1:11">
-      <c r="A83" t="s">
-        <v>27</v>
-      </c>
-      <c r="B83" t="s">
-        <v>109</v>
-      </c>
-      <c r="C83">
-        <v>57472</v>
-      </c>
-      <c r="D83">
-        <v>52851</v>
-      </c>
-      <c r="E83">
-        <v>216</v>
-      </c>
-      <c r="F83">
-        <v>2104</v>
-      </c>
-      <c r="G83">
-        <v>37189</v>
-      </c>
-      <c r="H83">
-        <v>248</v>
-      </c>
-      <c r="I83">
-        <v>74</v>
-      </c>
-      <c r="J83">
-        <v>351</v>
-      </c>
-      <c r="K83">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>27</v>
       </c>
       <c r="B84" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C84">
-        <v>35664</v>
+        <v>57472</v>
       </c>
       <c r="D84">
-        <v>67337</v>
+        <v>52851</v>
       </c>
       <c r="E84">
-        <v>311</v>
+        <v>216</v>
       </c>
       <c r="F84">
-        <v>694</v>
+        <v>2104</v>
       </c>
       <c r="G84">
-        <v>46165</v>
+        <v>37189</v>
       </c>
       <c r="H84">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="I84">
-        <v>15</v>
+        <v>74</v>
       </c>
       <c r="J84">
-        <v>168</v>
+        <v>351</v>
       </c>
       <c r="K84">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>27</v>
       </c>
       <c r="B85" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C85">
-        <v>11620</v>
+        <v>35664</v>
       </c>
       <c r="D85">
-        <v>10567</v>
+        <v>67337</v>
       </c>
       <c r="E85">
-        <v>77</v>
+        <v>311</v>
       </c>
       <c r="F85">
-        <v>235</v>
+        <v>694</v>
       </c>
       <c r="G85">
-        <v>5076</v>
+        <v>46165</v>
       </c>
       <c r="H85">
-        <v>107</v>
+        <v>262</v>
       </c>
       <c r="I85">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="J85">
-        <v>50</v>
+        <v>168</v>
       </c>
       <c r="K85">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>27</v>
       </c>
       <c r="B86" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C86">
-        <v>54034</v>
+        <v>11620</v>
       </c>
       <c r="D86">
-        <v>24315</v>
+        <v>10567</v>
       </c>
       <c r="E86">
-        <v>182</v>
+        <v>77</v>
       </c>
       <c r="F86">
-        <v>2537</v>
+        <v>235</v>
       </c>
       <c r="G86">
-        <v>24816</v>
+        <v>5076</v>
       </c>
       <c r="H86">
-        <v>239</v>
+        <v>107</v>
       </c>
       <c r="I86">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="J86">
-        <v>136</v>
+        <v>50</v>
       </c>
       <c r="K86">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>27</v>
       </c>
       <c r="B87" t="s">
+        <v>112</v>
+      </c>
+      <c r="C87">
+        <v>54034</v>
+      </c>
+      <c r="D87">
+        <v>24315</v>
+      </c>
+      <c r="E87">
+        <v>182</v>
+      </c>
+      <c r="F87">
+        <v>2537</v>
+      </c>
+      <c r="G87">
+        <v>24816</v>
+      </c>
+      <c r="H87">
+        <v>239</v>
+      </c>
+      <c r="I87">
+        <v>35</v>
+      </c>
+      <c r="J87">
+        <v>136</v>
+      </c>
+      <c r="K87">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>27</v>
+      </c>
+      <c r="B88" t="s">
         <v>113</v>
       </c>
-      <c r="C87">
+      <c r="C88">
         <v>33108</v>
       </c>
-      <c r="D87">
+      <c r="D88">
         <v>41769</v>
       </c>
-      <c r="E87">
+      <c r="E88">
         <v>67</v>
       </c>
-      <c r="F87">
+      <c r="F88">
         <v>2581</v>
       </c>
-      <c r="G87">
+      <c r="G88">
         <v>49821</v>
       </c>
-      <c r="H87">
+      <c r="H88">
         <v>139</v>
       </c>
-      <c r="I87">
+      <c r="I88">
         <v>13</v>
       </c>
-      <c r="J87">
+      <c r="J88">
         <v>110</v>
       </c>
-      <c r="K87">
+      <c r="K88">
         <v>68</v>
       </c>
     </row>

</xml_diff>